<commit_message>
worked on lab 2
</commit_message>
<xml_diff>
--- a/lab2/assignment1/martin/data/samples.xlsx
+++ b/lab2/assignment1/martin/data/samples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sciion\Documents\GitHub\TDDE01\lab2\assignment1\martin\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sciion\Sources\TDDE01\lab2\assignment1\martin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -362,12 +362,12 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,7 +387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -404,10 +404,10 @@
         <v>5</v>
       </c>
       <c r="F2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -424,10 +424,10 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -444,10 +444,10 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -464,10 +464,10 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -484,10 +484,10 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -504,10 +504,10 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -524,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>